<commit_message>
feat: Make Barcode optional and add Cantitatea column mapping
- Make Barcode field optional throughout the app
- Allow products to be imported/created without barcodes
- Enable barcode editing in EditProductDialog when empty
- Add "Cantitatea" column mapping for original xlsx files
- Update test xlsx file to use original column structure
- Add translation key for barcode help text

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/magazinOne.xlsx
+++ b/public/magazinOne.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:Q3"/>
+  <dimension ref="A2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -527,36 +527,6 @@
           <t>Cost preț magazin 100%</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>Cod de bare (Barcode)</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>Categorie</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>Stock curent</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>Stock minim</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>Furnizor</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>Data expirare</t>
-        </is>
-      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="2" t="n">
@@ -593,32 +563,6 @@
       </c>
       <c r="K3" s="4" t="n">
         <v>6.42</v>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>5901234567890</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>Conserve</t>
-        </is>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="P3" s="5" t="inlineStr">
-        <is>
-          <t>Riga Foods SRL</t>
-        </is>
-      </c>
-      <c r="Q3" s="2" t="inlineStr">
-        <is>
-          <t>2025-06-15</t>
-        </is>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1"/>

</xml_diff>